<commit_message>
expand test data:  - URI as "super" of a resource  - properties.xlsx: hasLinkTo: Resource, Region, StillImageRepresentation, AudioRepresentation, MovingImageRepresentation, ArchiveRepresentation
</commit_message>
<xml_diff>
--- a/testdata/excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json_files/test-name (test_label)/properties.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/excel2project_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171E5CDE-BBD6-F543-8B28-7223B83899F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7493FC4C-916B-2F46-9795-7DAF5EF5AA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="151">
   <si>
     <t>super</t>
   </si>
@@ -435,6 +435,57 @@
   </si>
   <si>
     <t>hasSequenceBounds</t>
+  </si>
+  <si>
+    <t>linkstoRegion</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Links to a region of an image</t>
+  </si>
+  <si>
+    <t>Verweist auf eine Region in einem Bild</t>
+  </si>
+  <si>
+    <t>Se réfère à une région d’une image</t>
+  </si>
+  <si>
+    <t>numprops: 1</t>
+  </si>
+  <si>
+    <t>hasLinkToImage</t>
+  </si>
+  <si>
+    <t>StillImageRepresentation</t>
+  </si>
+  <si>
+    <t>link to image</t>
+  </si>
+  <si>
+    <t>hasLinkToResource</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>hasLinkToArchiveRepresentation</t>
+  </si>
+  <si>
+    <t>ArchiveRepresentation</t>
+  </si>
+  <si>
+    <t>hasLinkToMovingImageRepesentation</t>
+  </si>
+  <si>
+    <t>MovingImageRepresentation</t>
+  </si>
+  <si>
+    <t>hasLinkToAudioRepesentation</t>
+  </si>
+  <si>
+    <t>AudioRepresentation</t>
   </si>
 </sst>
 </file>
@@ -836,9 +887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD25"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1598,44 +1649,126 @@
         <v>131</v>
       </c>
     </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="N21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="N24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>147</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>108</v>
       </c>
+      <c r="N25" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>13</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>108</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: bugs in json schema (DEV-1142) (#252)
 - resources-only.json: add "Region" and "Representation" as base resources
 - define super-resource in a non-recurring way
 - harmonization between all 4 schema files
 - improve: "format": "uri" has no effect --> needs a regex
 - expand test data:
    - URI as "super" of a resource
    - properties.xlsx: hasLinkTo: Resource, Region, StillImageRepresentation, AudioRepresentation, MovingImageRepresentation, ArchiveRepresentation
 - remove excelfileref
 - disallow nested excelfolderref: must be on top hierarchy level
 - remove redundancy of definitions/label, definitions/comment, definitions/description
 - langstring: make at least one language mandatory
 - take URI into account in the conditions for the super-properties
</commit_message>
<xml_diff>
--- a/testdata/excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json_files/test-name (test_label)/properties.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/excel2project_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171E5CDE-BBD6-F543-8B28-7223B83899F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34627E8-04E2-3D44-9FE2-DFCCEA7A8D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="149">
   <si>
     <t>super</t>
   </si>
@@ -435,6 +435,51 @@
   </si>
   <si>
     <t>hasSequenceBounds</t>
+  </si>
+  <si>
+    <t>linkstoRegion</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Links to a region of an image</t>
+  </si>
+  <si>
+    <t>numprops: 1</t>
+  </si>
+  <si>
+    <t>hasLinkToImage</t>
+  </si>
+  <si>
+    <t>StillImageRepresentation</t>
+  </si>
+  <si>
+    <t>link to image</t>
+  </si>
+  <si>
+    <t>hasLinkToResource</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>hasLinkToArchiveRepresentation</t>
+  </si>
+  <si>
+    <t>ArchiveRepresentation</t>
+  </si>
+  <si>
+    <t>hasLinkToMovingImageRepesentation</t>
+  </si>
+  <si>
+    <t>MovingImageRepresentation</t>
+  </si>
+  <si>
+    <t>hasLinkToAudioRepesentation</t>
+  </si>
+  <si>
+    <t>AudioRepresentation</t>
   </si>
 </sst>
 </file>
@@ -836,9 +881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD25"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1598,44 +1643,120 @@
         <v>131</v>
       </c>
     </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="N21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="N24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>145</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>108</v>
       </c>
+      <c r="N25" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>13</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>108</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>